<commit_message>
Adição de novas colunas para controle de versão de pedidos.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/leitorcartao.xlsx
+++ b/Hardware/BOM/leitorcartao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="383">
   <si>
     <t>Part</t>
   </si>
@@ -1157,6 +1157,12 @@
   </si>
   <si>
     <t>FSK_PN</t>
+  </si>
+  <si>
+    <t>FSK</t>
+  </si>
+  <si>
+    <t>PSK</t>
   </si>
 </sst>
 </file>
@@ -1974,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K162"/>
+  <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1991,7 +1997,7 @@
     <col min="9" max="9" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2025,8 +2031,20 @@
       <c r="K1" s="2" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2051,7 +2069,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2078,7 +2096,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2103,7 +2121,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -2130,7 +2148,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2175,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2184,7 +2202,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -2211,7 +2229,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -2238,7 +2256,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -2265,7 +2283,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -2292,7 +2310,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -2319,7 +2337,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -2346,7 +2364,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -2373,7 +2391,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -2400,7 +2418,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>

</xml_diff>